<commit_message>
Fixed critical mistake in SimDataProcessing.py: attraction utilities was not sorted by attraction index
</commit_message>
<xml_diff>
--- a/slvr/Database/Intrinsic Utility.xlsx
+++ b/slvr/Database/Intrinsic Utility.xlsx
@@ -1,20 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10609"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11208"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/gary/Dropbox/tourism survey/Database/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/gary/Dropbox/City Tourism Estimation/slvr/Database/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2234A873-B03D-234B-B930-916C8ACAB04F}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7504891A-B464-6543-BD6E-FF213CCE9916}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-20" yWindow="0" windowWidth="28800" windowHeight="18000" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Intrinsic Utility" sheetId="1" r:id="rId1"/>
-    <sheet name="data" sheetId="2" r:id="rId2"/>
+    <sheet name="idx &amp; name" sheetId="3" r:id="rId2"/>
+    <sheet name="data" sheetId="4" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -29,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="105" uniqueCount="62">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="220" uniqueCount="65">
   <si>
     <t>Area code</t>
   </si>
@@ -215,12 +216,21 @@
   </si>
   <si>
     <t>gourmet</t>
+  </si>
+  <si>
+    <t>Area index</t>
+  </si>
+  <si>
+    <t>Column1</t>
+  </si>
+  <si>
+    <t>Column2</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr9="http://schemas.microsoft.com/office/spreadsheetml/2016/revision9" mc:Ignorable="x14ac x16r2 xr xr9">
   <fonts count="21">
     <font>
       <sz val="12"/>
@@ -376,7 +386,7 @@
       <name val="Calibri (Body)"/>
     </font>
   </fonts>
-  <fills count="33">
+  <fills count="34">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -554,6 +564,12 @@
       <patternFill patternType="solid">
         <fgColor theme="9" tint="0.39997558519241921"/>
         <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.14999847407452621"/>
+        <bgColor theme="0" tint="-0.14999847407452621"/>
       </patternFill>
     </fill>
   </fills>
@@ -866,7 +882,7 @@
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="10" xfId="42" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
@@ -895,6 +911,15 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -907,14 +932,11 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="18" fillId="33" borderId="10" xfId="42" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="10" xfId="42" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="43">
@@ -962,63 +984,7 @@
     <cellStyle name="Warning Text" xfId="14" builtinId="11" customBuiltin="1"/>
     <cellStyle name="標準_M_手段場所code" xfId="42" xr:uid="{F28D13A7-3967-5146-B32A-E01CF23EDF6C}"/>
   </cellStyles>
-  <dxfs count="8">
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top/>
-        <bottom/>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <border diagonalUp="0" diagonalDown="0">
-        <left/>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top/>
-        <bottom/>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right/>
-        <top/>
-        <bottom/>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="thin">
-          <color indexed="22"/>
-        </left>
-        <right style="thin">
-          <color indexed="22"/>
-        </right>
-        <top style="thin">
-          <color indexed="22"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="22"/>
-        </bottom>
-      </border>
-    </dxf>
+  <dxfs count="4">
     <dxf>
       <numFmt numFmtId="0" formatCode="General"/>
       <border diagonalUp="0" diagonalDown="0">
@@ -1076,7 +1042,9 @@
       </border>
     </dxf>
   </dxfs>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <tableStyles count="1" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16">
+    <tableStyle name="Table Style 1" pivot="0" count="0" xr9:uid="{E980C99C-8EE2-094F-B30D-C535DA3FD8CC}"/>
+  </tableStyles>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -1178,7 +1146,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>'Intrinsic Utility'!$B$1</c:f>
+              <c:f>'Intrinsic Utility'!$C$1</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -1255,7 +1223,7 @@
           </c:dLbls>
           <c:cat>
             <c:strRef>
-              <c:f>'Intrinsic Utility'!$A$2:$A$38</c:f>
+              <c:f>'Intrinsic Utility'!$B$2:$B$38</c:f>
               <c:strCache>
                 <c:ptCount val="37"/>
                 <c:pt idx="0">
@@ -1374,7 +1342,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'Intrinsic Utility'!$B$2:$B$38</c:f>
+              <c:f>'Intrinsic Utility'!$C$2:$C$38</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="37"/>
@@ -1503,7 +1471,7 @@
           <c:order val="1"/>
           <c:tx>
             <c:strRef>
-              <c:f>'Intrinsic Utility'!$C$1</c:f>
+              <c:f>'Intrinsic Utility'!$D$1</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -1580,7 +1548,7 @@
           </c:dLbls>
           <c:cat>
             <c:strRef>
-              <c:f>'Intrinsic Utility'!$A$2:$A$38</c:f>
+              <c:f>'Intrinsic Utility'!$B$2:$B$38</c:f>
               <c:strCache>
                 <c:ptCount val="37"/>
                 <c:pt idx="0">
@@ -1699,7 +1667,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'Intrinsic Utility'!$C$2:$C$38</c:f>
+              <c:f>'Intrinsic Utility'!$D$2:$D$38</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="37"/>
@@ -1828,7 +1796,7 @@
           <c:order val="2"/>
           <c:tx>
             <c:strRef>
-              <c:f>'Intrinsic Utility'!$D$1</c:f>
+              <c:f>'Intrinsic Utility'!$E$1</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -1905,7 +1873,7 @@
           </c:dLbls>
           <c:cat>
             <c:strRef>
-              <c:f>'Intrinsic Utility'!$A$2:$A$38</c:f>
+              <c:f>'Intrinsic Utility'!$B$2:$B$38</c:f>
               <c:strCache>
                 <c:ptCount val="37"/>
                 <c:pt idx="0">
@@ -2024,7 +1992,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'Intrinsic Utility'!$D$2:$D$38</c:f>
+              <c:f>'Intrinsic Utility'!$E$2:$E$38</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="37"/>
@@ -2908,13 +2876,13 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>6</xdr:col>
+      <xdr:col>7</xdr:col>
       <xdr:colOff>0</xdr:colOff>
       <xdr:row>0</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>14</xdr:col>
+      <xdr:col>15</xdr:col>
       <xdr:colOff>33867</xdr:colOff>
       <xdr:row>38</xdr:row>
       <xdr:rowOff>16933</xdr:rowOff>
@@ -2946,13 +2914,13 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>15</xdr:col>
+      <xdr:col>16</xdr:col>
       <xdr:colOff>0</xdr:colOff>
       <xdr:row>12</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>18</xdr:col>
+      <xdr:col>19</xdr:col>
       <xdr:colOff>457200</xdr:colOff>
       <xdr:row>17</xdr:row>
       <xdr:rowOff>179493</xdr:rowOff>
@@ -3170,17 +3138,17 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{5EAADAD5-07C1-1347-8AA0-B75D200C4B5B}" name="Table1" displayName="Table1" ref="A1:E38" totalsRowShown="0">
-  <autoFilter ref="A1:E38" xr:uid="{E9C523DD-C198-F34A-80C9-20ACAFBDEF4B}"/>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:E38">
-    <sortCondition descending="1" ref="E1:E38"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{5EAADAD5-07C1-1347-8AA0-B75D200C4B5B}" name="Table1" displayName="Table1" ref="B1:F38" totalsRowShown="0">
+  <autoFilter ref="B1:F38" xr:uid="{E9C523DD-C198-F34A-80C9-20ACAFBDEF4B}"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="B2:F38">
+    <sortCondition descending="1" ref="F1:F38"/>
   </sortState>
   <tableColumns count="5">
-    <tableColumn id="1" xr3:uid="{524AB209-8F36-0146-8D72-7293B9F2450E}" name="Area code" dataDxfId="7" dataCellStyle="標準_M_手段場所code"/>
-    <tableColumn id="2" xr3:uid="{114D5D97-BE0E-2A42-8EEC-AAE15B8B511B}" name="red leaves, temple and shrines" dataDxfId="6"/>
+    <tableColumn id="1" xr3:uid="{524AB209-8F36-0146-8D72-7293B9F2450E}" name="Area code" dataDxfId="3" dataCellStyle="標準_M_手段場所code"/>
+    <tableColumn id="2" xr3:uid="{114D5D97-BE0E-2A42-8EEC-AAE15B8B511B}" name="red leaves, temple and shrines" dataDxfId="2"/>
     <tableColumn id="3" xr3:uid="{502FFF75-959B-8846-B275-DE952377419D}" name="gourmet"/>
-    <tableColumn id="4" xr3:uid="{799F3E4D-E9AA-0E49-87C6-2027FBAC8A5D}" name="leisure activities" dataDxfId="5"/>
-    <tableColumn id="5" xr3:uid="{B82F4906-276B-6644-9C32-65BD0A9DE19D}" name="total" dataDxfId="4">
+    <tableColumn id="4" xr3:uid="{799F3E4D-E9AA-0E49-87C6-2027FBAC8A5D}" name="leisure activities" dataDxfId="1"/>
+    <tableColumn id="5" xr3:uid="{B82F4906-276B-6644-9C32-65BD0A9DE19D}" name="total" dataDxfId="0">
       <calculatedColumnFormula>SUM(Table1[[#This Row],[red leaves, temple and shrines]:[leisure activities]])</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -3189,21 +3157,31 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{FE388A54-11A3-5F48-BCC0-391E5EFA395C}" name="Table13" displayName="Table13" ref="A1:E38" totalsRowShown="0">
-  <autoFilter ref="A1:E38" xr:uid="{CBD35E7C-FCCD-5A47-A022-574249EF06BB}"/>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:E38">
-    <sortCondition descending="1" ref="E1:E38"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{147A9A0C-91B7-2149-835E-6CF7C9550885}" name="Table4" displayName="Table4" ref="B1:C38" totalsRowShown="0">
+  <autoFilter ref="B1:C38" xr:uid="{E21F013F-09B6-3A45-9378-4C2118D787F6}"/>
+  <tableColumns count="2">
+    <tableColumn id="1" xr3:uid="{67207FE3-DFDD-5541-93CD-2995D406A3A9}" name="Column1"/>
+    <tableColumn id="2" xr3:uid="{6570AA89-28E5-5C4A-AB37-7791D6019A00}" name="Column2"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium4" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{5BE45205-9FA9-FD45-8F31-ACF7EEAC07FE}" name="Table6" displayName="Table6" ref="A1:F38" totalsRowShown="0">
+  <autoFilter ref="A1:F38" xr:uid="{565B8E54-DB48-DF47-8001-6CD01419C924}"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:F38">
+    <sortCondition ref="A1:A38"/>
   </sortState>
-  <tableColumns count="5">
-    <tableColumn id="1" xr3:uid="{7F54AC16-D4D0-C14F-9BF1-4148342C40AA}" name="Area code" dataDxfId="3" dataCellStyle="標準_M_手段場所code"/>
-    <tableColumn id="2" xr3:uid="{1B3F2048-F48E-5443-9211-E5DE4C1F43D2}" name="red leaves, temple and shrines" dataDxfId="2"/>
-    <tableColumn id="3" xr3:uid="{32050F8D-225C-3845-B69B-F788359D7C75}" name="gourmet"/>
-    <tableColumn id="4" xr3:uid="{8144D118-EBA3-2F45-A8C8-5C3A67E89DAD}" name="leisure activities" dataDxfId="1"/>
-    <tableColumn id="5" xr3:uid="{333F33B1-80C8-7E4B-A3F2-B665B2AEE174}" name="total" dataDxfId="0">
-      <calculatedColumnFormula>SUM(Table13[[#This Row],[red leaves, temple and shrines]:[leisure activities]])</calculatedColumnFormula>
-    </tableColumn>
+  <tableColumns count="6">
+    <tableColumn id="1" xr3:uid="{DEE7877F-1EBC-854A-8BF5-5742F73088BA}" name="Area index"/>
+    <tableColumn id="2" xr3:uid="{BD0591F9-14CB-F44F-A6AA-7F6BA9470DAB}" name="Area code"/>
+    <tableColumn id="3" xr3:uid="{0AA38292-577D-AC49-A2EE-5997CEFB725E}" name="red leaves, temple and shrines"/>
+    <tableColumn id="4" xr3:uid="{BD5144FA-19BD-4A43-99B7-E6BD41303A2A}" name="gourmet"/>
+    <tableColumn id="5" xr3:uid="{9B10C1E2-BD57-E440-BA16-EFD092BE77CA}" name="leisure activities"/>
+    <tableColumn id="6" xr3:uid="{EF5EB4C6-B702-0844-9008-CF8FB024BAA0}" name="total"/>
   </tableColumns>
-  <tableStyleInfo name="TableStyleMedium21" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+  <tableStyleInfo name="TableStyleMedium4" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
@@ -3504,841 +3482,1362 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:T38"/>
+  <dimension ref="A1:U79"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="168" workbookViewId="0">
-      <selection sqref="A1:E38"/>
+    <sheetView topLeftCell="A23" zoomScaleNormal="168" workbookViewId="0">
+      <selection activeCell="F43" sqref="F43:F79"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
   <cols>
-    <col min="1" max="1" width="17" customWidth="1"/>
+    <col min="2" max="2" width="17" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:20" ht="17" thickBot="1">
+    <row r="1" spans="1:21" ht="17" thickBot="1">
       <c r="A1" t="s">
+        <v>62</v>
+      </c>
+      <c r="B1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C1" t="s">
         <v>60</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>61</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>50</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>59</v>
       </c>
-      <c r="F1" s="7"/>
       <c r="G1" s="7"/>
       <c r="H1" s="7"/>
       <c r="I1" s="7"/>
       <c r="J1" s="7"/>
-      <c r="K1" s="8"/>
+      <c r="K1" s="7"/>
       <c r="L1" s="8"/>
-    </row>
-    <row r="2" spans="1:20">
-      <c r="A2" s="1" t="s">
+      <c r="M1" s="8"/>
+    </row>
+    <row r="2" spans="1:21">
+      <c r="B2" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="B2" s="2">
+      <c r="C2" s="2">
         <v>0.76629066303512905</v>
       </c>
-      <c r="C2">
+      <c r="D2">
         <v>0.843982451523971</v>
       </c>
-      <c r="D2" s="3">
+      <c r="E2" s="3">
         <v>0.89736915738711498</v>
       </c>
-      <c r="E2" s="9">
+      <c r="F2" s="9">
         <f>SUM(Table1[[#This Row],[red leaves, temple and shrines]:[leisure activities]])</f>
         <v>2.507642271946215</v>
       </c>
-      <c r="P2" s="4" t="s">
+      <c r="Q2" s="4" t="s">
         <v>38</v>
       </c>
-      <c r="Q2" s="12" t="s">
+      <c r="R2" s="15" t="s">
         <v>39</v>
       </c>
-      <c r="R2" s="12"/>
-      <c r="S2" s="12" t="s">
+      <c r="S2" s="15"/>
+      <c r="T2" s="15" t="s">
         <v>40</v>
       </c>
-      <c r="T2" s="13"/>
-    </row>
-    <row r="3" spans="1:20">
-      <c r="A3" s="1" t="s">
+      <c r="U2" s="16"/>
+    </row>
+    <row r="3" spans="1:21">
+      <c r="B3" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="B3" s="2">
+      <c r="C3" s="2">
         <v>0.69480038130807198</v>
       </c>
-      <c r="C3">
+      <c r="D3">
         <v>0.63404031916133596</v>
       </c>
-      <c r="D3" s="3">
+      <c r="E3" s="3">
         <v>0.79998075483900299</v>
       </c>
-      <c r="E3" s="9">
+      <c r="F3" s="9">
         <f>SUM(Table1[[#This Row],[red leaves, temple and shrines]:[leisure activities]])</f>
         <v>2.1288214553084108</v>
       </c>
-      <c r="P3" s="5">
+      <c r="Q3" s="5">
         <v>1</v>
       </c>
-      <c r="Q3" s="14" t="s">
+      <c r="R3" s="17" t="s">
         <v>41</v>
       </c>
-      <c r="R3" s="14"/>
-      <c r="S3" s="14" t="s">
+      <c r="S3" s="17"/>
+      <c r="T3" s="17" t="s">
         <v>42</v>
       </c>
-      <c r="T3" s="15"/>
-    </row>
-    <row r="4" spans="1:20">
-      <c r="A4" s="1" t="s">
+      <c r="U3" s="18"/>
+    </row>
+    <row r="4" spans="1:21">
+      <c r="B4" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="B4" s="2">
+      <c r="C4" s="2">
         <v>0.38773301736600302</v>
       </c>
-      <c r="C4">
+      <c r="D4">
         <v>1</v>
       </c>
-      <c r="D4" s="3">
+      <c r="E4" s="3">
         <v>0.72222222222222199</v>
       </c>
-      <c r="E4" s="9">
+      <c r="F4" s="9">
         <f>SUM(Table1[[#This Row],[red leaves, temple and shrines]:[leisure activities]])</f>
         <v>2.1099552395882251</v>
       </c>
-      <c r="P4" s="5">
+      <c r="Q4" s="5">
         <v>2</v>
       </c>
-      <c r="Q4" s="10" t="s">
+      <c r="R4" s="10" t="s">
         <v>43</v>
       </c>
-      <c r="R4" s="10"/>
-      <c r="S4" s="10" t="s">
+      <c r="S4" s="10"/>
+      <c r="T4" s="10" t="s">
         <v>44</v>
       </c>
-      <c r="T4" s="11"/>
-    </row>
-    <row r="5" spans="1:20">
-      <c r="A5" s="1" t="s">
+      <c r="U4" s="11"/>
+    </row>
+    <row r="5" spans="1:21">
+      <c r="B5" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="B5" s="2">
+      <c r="C5" s="2">
         <v>0.75886464920609997</v>
       </c>
-      <c r="C5">
+      <c r="D5">
         <v>0.66597361433972002</v>
       </c>
-      <c r="D5" s="3">
+      <c r="E5" s="3">
         <v>0.46840330674714598</v>
       </c>
-      <c r="E5" s="9">
+      <c r="F5" s="9">
         <f>SUM(Table1[[#This Row],[red leaves, temple and shrines]:[leisure activities]])</f>
         <v>1.8932415702929661</v>
       </c>
-      <c r="P5" s="5">
+      <c r="Q5" s="5">
         <v>3</v>
       </c>
-      <c r="Q5" s="10" t="s">
+      <c r="R5" s="10" t="s">
         <v>45</v>
       </c>
-      <c r="R5" s="10"/>
-      <c r="S5" s="10" t="s">
+      <c r="S5" s="10"/>
+      <c r="T5" s="10" t="s">
         <v>46</v>
       </c>
-      <c r="T5" s="11"/>
-    </row>
-    <row r="6" spans="1:20">
-      <c r="A6" s="1" t="s">
+      <c r="U5" s="11"/>
+    </row>
+    <row r="6" spans="1:21">
+      <c r="B6" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="B6" s="2">
+      <c r="C6" s="2">
         <v>0.49281036074163298</v>
       </c>
-      <c r="C6">
+      <c r="D6">
         <v>0.75070339259594698</v>
       </c>
-      <c r="D6" s="3">
+      <c r="E6" s="3">
         <v>0.61263215833006002</v>
       </c>
-      <c r="E6" s="9">
+      <c r="F6" s="9">
         <f>SUM(Table1[[#This Row],[red leaves, temple and shrines]:[leisure activities]])</f>
         <v>1.85614591166764</v>
       </c>
-      <c r="P6" s="5">
+      <c r="Q6" s="5">
         <v>4</v>
       </c>
-      <c r="Q6" s="10" t="s">
+      <c r="R6" s="10" t="s">
         <v>47</v>
       </c>
-      <c r="R6" s="10"/>
-      <c r="S6" s="10" t="s">
+      <c r="S6" s="10"/>
+      <c r="T6" s="10" t="s">
         <v>48</v>
       </c>
-      <c r="T6" s="11"/>
-    </row>
-    <row r="7" spans="1:20">
-      <c r="A7" s="1" t="s">
+      <c r="U6" s="11"/>
+    </row>
+    <row r="7" spans="1:21">
+      <c r="B7" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="B7" s="2">
+      <c r="C7" s="2">
         <v>0.647873331891062</v>
       </c>
-      <c r="C7">
+      <c r="D7">
         <v>0.58974668591095603</v>
       </c>
-      <c r="D7" s="3">
+      <c r="E7" s="3">
         <v>0.61134561956866995</v>
       </c>
-      <c r="E7" s="9">
+      <c r="F7" s="9">
         <f>SUM(Table1[[#This Row],[red leaves, temple and shrines]:[leisure activities]])</f>
         <v>1.848965637370688</v>
       </c>
-      <c r="P7" s="5">
+      <c r="Q7" s="5">
         <v>5</v>
       </c>
-      <c r="Q7" s="10" t="s">
+      <c r="R7" s="10" t="s">
         <v>49</v>
       </c>
-      <c r="R7" s="10"/>
-      <c r="S7" s="16" t="s">
+      <c r="S7" s="10"/>
+      <c r="T7" s="14" t="s">
         <v>50</v>
       </c>
-      <c r="T7" s="11"/>
-    </row>
-    <row r="8" spans="1:20">
-      <c r="A8" s="1" t="s">
+      <c r="U7" s="11"/>
+    </row>
+    <row r="8" spans="1:21">
+      <c r="B8" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="B8" s="2">
+      <c r="C8" s="2">
         <v>0.86517596384200002</v>
       </c>
-      <c r="C8">
+      <c r="D8">
         <v>0.44741290079132801</v>
       </c>
-      <c r="D8" s="3">
+      <c r="E8" s="3">
         <v>0.36182313565826102</v>
       </c>
-      <c r="E8" s="9">
+      <c r="F8" s="9">
         <f>SUM(Table1[[#This Row],[red leaves, temple and shrines]:[leisure activities]])</f>
         <v>1.674412000291589</v>
       </c>
-      <c r="P8" s="5">
+      <c r="Q8" s="5">
         <v>6</v>
       </c>
-      <c r="Q8" s="10" t="s">
+      <c r="R8" s="10" t="s">
         <v>51</v>
       </c>
-      <c r="R8" s="10"/>
-      <c r="S8" s="10" t="s">
+      <c r="S8" s="10"/>
+      <c r="T8" s="10" t="s">
         <v>52</v>
       </c>
-      <c r="T8" s="11"/>
-    </row>
-    <row r="9" spans="1:20">
-      <c r="A9" s="1" t="s">
+      <c r="U8" s="11"/>
+    </row>
+    <row r="9" spans="1:21">
+      <c r="B9" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="B9" s="2">
+      <c r="C9" s="2">
         <v>0.84804120995904297</v>
       </c>
-      <c r="C9">
+      <c r="D9">
         <v>0.42419964013700601</v>
       </c>
-      <c r="D9" s="3">
+      <c r="E9" s="3">
         <v>0.31932294062842798</v>
       </c>
-      <c r="E9" s="9">
+      <c r="F9" s="9">
         <f>SUM(Table1[[#This Row],[red leaves, temple and shrines]:[leisure activities]])</f>
         <v>1.5915637907244768</v>
       </c>
-      <c r="P9" s="5">
+      <c r="Q9" s="5">
         <v>7</v>
       </c>
-      <c r="Q9" s="10" t="s">
+      <c r="R9" s="10" t="s">
         <v>53</v>
       </c>
-      <c r="R9" s="10"/>
-      <c r="S9" s="10" t="s">
+      <c r="S9" s="10"/>
+      <c r="T9" s="10" t="s">
         <v>54</v>
       </c>
-      <c r="T9" s="11"/>
-    </row>
-    <row r="10" spans="1:20">
-      <c r="A10" s="1" t="s">
+      <c r="U9" s="11"/>
+    </row>
+    <row r="10" spans="1:21">
+      <c r="B10" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="B10" s="2">
+      <c r="C10" s="2">
         <v>0.84559953924055298</v>
       </c>
-      <c r="C10">
+      <c r="D10">
         <v>0.311859991058062</v>
       </c>
-      <c r="D10" s="3">
+      <c r="E10" s="3">
         <v>0.39136496828702</v>
       </c>
-      <c r="E10" s="9">
+      <c r="F10" s="9">
         <f>SUM(Table1[[#This Row],[red leaves, temple and shrines]:[leisure activities]])</f>
         <v>1.548824498585635</v>
       </c>
-      <c r="P10" s="5">
+      <c r="Q10" s="5">
         <v>8</v>
       </c>
-      <c r="Q10" s="10" t="s">
+      <c r="R10" s="10" t="s">
         <v>55</v>
       </c>
-      <c r="R10" s="10"/>
-      <c r="S10" s="10" t="s">
+      <c r="S10" s="10"/>
+      <c r="T10" s="10" t="s">
         <v>56</v>
       </c>
-      <c r="T10" s="11"/>
-    </row>
-    <row r="11" spans="1:20" ht="17" thickBot="1">
-      <c r="A11" s="1" t="s">
+      <c r="U10" s="11"/>
+    </row>
+    <row r="11" spans="1:21" ht="17" thickBot="1">
+      <c r="B11" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="B11" s="2">
+      <c r="C11" s="2">
         <v>0.56018420706636796</v>
       </c>
-      <c r="C11">
+      <c r="D11">
         <v>0.464471120054052</v>
       </c>
-      <c r="D11" s="3">
+      <c r="E11" s="3">
         <v>0.412426532417553</v>
       </c>
-      <c r="E11" s="9">
+      <c r="F11" s="9">
         <f>SUM(Table1[[#This Row],[red leaves, temple and shrines]:[leisure activities]])</f>
         <v>1.4370818595379728</v>
       </c>
-      <c r="P11" s="6">
+      <c r="Q11" s="6">
         <v>9</v>
       </c>
-      <c r="Q11" s="17" t="s">
+      <c r="R11" s="12" t="s">
         <v>57</v>
       </c>
-      <c r="R11" s="17"/>
-      <c r="S11" s="17" t="s">
+      <c r="S11" s="12"/>
+      <c r="T11" s="12" t="s">
         <v>58</v>
       </c>
-      <c r="T11" s="18"/>
-    </row>
-    <row r="12" spans="1:20">
-      <c r="A12" s="1" t="s">
+      <c r="U11" s="13"/>
+    </row>
+    <row r="12" spans="1:21">
+      <c r="B12" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="B12" s="2">
+      <c r="C12" s="2">
         <v>0.49709465907878803</v>
       </c>
-      <c r="C12">
+      <c r="D12">
         <v>0.58630668172201905</v>
       </c>
-      <c r="D12" s="3">
+      <c r="E12" s="3">
         <v>0.321493232413396</v>
       </c>
-      <c r="E12" s="9">
+      <c r="F12" s="9">
         <f>SUM(Table1[[#This Row],[red leaves, temple and shrines]:[leisure activities]])</f>
         <v>1.4048945732142029</v>
       </c>
     </row>
-    <row r="13" spans="1:20">
-      <c r="A13" s="1" t="s">
+    <row r="13" spans="1:21">
+      <c r="B13" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="B13" s="2">
+      <c r="C13" s="2">
         <v>0.55196481794434304</v>
       </c>
-      <c r="C13">
+      <c r="D13">
         <v>0.46284931618652497</v>
       </c>
-      <c r="D13" s="3">
+      <c r="E13" s="3">
         <v>0.31691814038589999</v>
       </c>
-      <c r="E13" s="9">
+      <c r="F13" s="9">
         <f>SUM(Table1[[#This Row],[red leaves, temple and shrines]:[leisure activities]])</f>
         <v>1.3317322745167681</v>
       </c>
     </row>
-    <row r="14" spans="1:20">
-      <c r="A14" s="1" t="s">
+    <row r="14" spans="1:21">
+      <c r="B14" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="B14" s="2">
+      <c r="C14" s="2">
         <v>0.44372111837551997</v>
       </c>
-      <c r="C14">
+      <c r="D14">
         <v>0.38300956093350202</v>
       </c>
-      <c r="D14" s="3">
+      <c r="E14" s="3">
         <v>0.48815989908006302</v>
       </c>
-      <c r="E14" s="9">
+      <c r="F14" s="9">
         <f>SUM(Table1[[#This Row],[red leaves, temple and shrines]:[leisure activities]])</f>
         <v>1.314890578389085</v>
       </c>
     </row>
-    <row r="15" spans="1:20">
-      <c r="A15" s="1" t="s">
+    <row r="15" spans="1:21">
+      <c r="B15" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="B15" s="2">
+      <c r="C15" s="2">
         <v>0.21905617666692601</v>
       </c>
-      <c r="C15">
+      <c r="D15">
         <v>0.60518310130615205</v>
       </c>
-      <c r="D15" s="3">
+      <c r="E15" s="3">
         <v>0.38155003332135501</v>
       </c>
-      <c r="E15" s="9">
+      <c r="F15" s="9">
         <f>SUM(Table1[[#This Row],[red leaves, temple and shrines]:[leisure activities]])</f>
         <v>1.2057893112944331</v>
       </c>
     </row>
-    <row r="16" spans="1:20">
-      <c r="A16" s="1" t="s">
+    <row r="16" spans="1:21">
+      <c r="B16" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="B16" s="2">
+      <c r="C16" s="2">
         <v>0.50735715650678304</v>
       </c>
-      <c r="C16">
+      <c r="D16">
         <v>0.39824190544420501</v>
       </c>
-      <c r="D16" s="3">
+      <c r="E16" s="3">
         <v>0.29802686804033601</v>
       </c>
-      <c r="E16" s="9">
+      <c r="F16" s="9">
         <f>SUM(Table1[[#This Row],[red leaves, temple and shrines]:[leisure activities]])</f>
         <v>1.2036259299913241</v>
       </c>
     </row>
-    <row r="17" spans="1:5">
-      <c r="A17" s="1" t="s">
+    <row r="17" spans="2:6">
+      <c r="B17" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="B17" s="2">
+      <c r="C17" s="2">
         <v>0.30180992114149102</v>
       </c>
-      <c r="C17">
+      <c r="D17">
         <v>0.51239449567655704</v>
       </c>
-      <c r="D17" s="3">
+      <c r="E17" s="3">
         <v>0.37959614652268803</v>
       </c>
-      <c r="E17" s="9">
+      <c r="F17" s="9">
         <f>SUM(Table1[[#This Row],[red leaves, temple and shrines]:[leisure activities]])</f>
         <v>1.193800563340736</v>
       </c>
     </row>
-    <row r="18" spans="1:5">
-      <c r="A18" s="1" t="s">
+    <row r="18" spans="2:6">
+      <c r="B18" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="B18" s="2">
+      <c r="C18" s="2">
         <v>0.387879268590961</v>
       </c>
-      <c r="C18">
+      <c r="D18">
         <v>0.48768257748393101</v>
       </c>
-      <c r="D18" s="3">
+      <c r="E18" s="3">
         <v>0.31691814038589999</v>
       </c>
-      <c r="E18" s="9">
+      <c r="F18" s="9">
         <f>SUM(Table1[[#This Row],[red leaves, temple and shrines]:[leisure activities]])</f>
         <v>1.192479986460792</v>
       </c>
     </row>
-    <row r="19" spans="1:5">
-      <c r="A19" s="1" t="s">
+    <row r="19" spans="2:6">
+      <c r="B19" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="B19" s="2">
+      <c r="C19" s="2">
         <v>0.42001622542966099</v>
       </c>
-      <c r="C19">
+      <c r="D19">
         <v>0.39348840239919097</v>
       </c>
-      <c r="D19" s="3">
+      <c r="E19" s="3">
         <v>0.36535124536022401</v>
       </c>
-      <c r="E19" s="9">
+      <c r="F19" s="9">
         <f>SUM(Table1[[#This Row],[red leaves, temple and shrines]:[leisure activities]])</f>
         <v>1.1788558731890761</v>
       </c>
     </row>
-    <row r="20" spans="1:5">
-      <c r="A20" s="1" t="s">
+    <row r="20" spans="2:6">
+      <c r="B20" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="B20" s="2">
+      <c r="C20" s="2">
         <v>0.59753013079116402</v>
       </c>
-      <c r="C20">
+      <c r="D20">
         <v>0.33326031055897498</v>
       </c>
-      <c r="D20" s="3">
+      <c r="E20" s="3">
         <v>0.22469830162035301</v>
       </c>
-      <c r="E20" s="9">
+      <c r="F20" s="9">
         <f>SUM(Table1[[#This Row],[red leaves, temple and shrines]:[leisure activities]])</f>
         <v>1.1554887429704921</v>
       </c>
     </row>
-    <row r="21" spans="1:5">
-      <c r="A21" s="1" t="s">
+    <row r="21" spans="2:6">
+      <c r="B21" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B21" s="2">
+      <c r="C21" s="2">
         <v>0.51750653091780496</v>
       </c>
-      <c r="C21">
+      <c r="D21">
         <v>0.36413314134936797</v>
       </c>
-      <c r="D21" s="3">
+      <c r="E21" s="3">
         <v>0.26376738507287201</v>
       </c>
-      <c r="E21" s="9">
+      <c r="F21" s="9">
         <f>SUM(Table1[[#This Row],[red leaves, temple and shrines]:[leisure activities]])</f>
         <v>1.1454070573400448</v>
       </c>
     </row>
-    <row r="22" spans="1:5">
-      <c r="A22" s="1" t="s">
+    <row r="22" spans="2:6">
+      <c r="B22" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="B22" s="2">
+      <c r="C22" s="2">
         <v>0.45841234955560201</v>
       </c>
-      <c r="C22">
+      <c r="D22">
         <v>0.42294676124438702</v>
       </c>
-      <c r="D22" s="3">
+      <c r="E22" s="3">
         <v>0.256194021047779</v>
       </c>
-      <c r="E22" s="9">
+      <c r="F22" s="9">
         <f>SUM(Table1[[#This Row],[red leaves, temple and shrines]:[leisure activities]])</f>
         <v>1.1375531318477679</v>
       </c>
     </row>
-    <row r="23" spans="1:5">
-      <c r="A23" s="1" t="s">
+    <row r="23" spans="2:6">
+      <c r="B23" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="B23" s="2">
+      <c r="C23" s="2">
         <v>0.531498341761096</v>
       </c>
-      <c r="C23">
+      <c r="D23">
         <v>0.287155135257879</v>
       </c>
-      <c r="D23" s="3">
+      <c r="E23" s="3">
         <v>0.30131542130644201</v>
       </c>
-      <c r="E23" s="9">
+      <c r="F23" s="9">
         <f>SUM(Table1[[#This Row],[red leaves, temple and shrines]:[leisure activities]])</f>
         <v>1.119968898325417</v>
       </c>
     </row>
-    <row r="24" spans="1:5">
-      <c r="A24" s="1" t="s">
+    <row r="24" spans="2:6">
+      <c r="B24" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="B24" s="2">
+      <c r="C24" s="2">
         <v>0.45001851657071301</v>
       </c>
-      <c r="C24">
+      <c r="D24">
         <v>0.32299738184833798</v>
       </c>
-      <c r="D24" s="3">
+      <c r="E24" s="3">
         <v>0.27088983565410402</v>
       </c>
-      <c r="E24" s="9">
+      <c r="F24" s="9">
         <f>SUM(Table1[[#This Row],[red leaves, temple and shrines]:[leisure activities]])</f>
         <v>1.043905734073155</v>
       </c>
     </row>
-    <row r="25" spans="1:5">
-      <c r="A25" s="1" t="s">
+    <row r="25" spans="2:6">
+      <c r="B25" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="B25" s="2">
+      <c r="C25" s="2">
         <v>0.45363652525970799</v>
       </c>
-      <c r="C25">
+      <c r="D25">
         <v>0.33632613060500299</v>
       </c>
-      <c r="D25" s="3">
+      <c r="E25" s="3">
         <v>0.24358957396591799</v>
       </c>
-      <c r="E25" s="9">
+      <c r="F25" s="9">
         <f>SUM(Table1[[#This Row],[red leaves, temple and shrines]:[leisure activities]])</f>
         <v>1.033552229830629</v>
       </c>
     </row>
-    <row r="26" spans="1:5">
-      <c r="A26" s="1" t="s">
+    <row r="26" spans="2:6">
+      <c r="B26" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="B26" s="2">
+      <c r="C26" s="2">
         <v>0.37021656663841301</v>
       </c>
-      <c r="C26">
+      <c r="D26">
         <v>0.37660286969005002</v>
       </c>
-      <c r="D26" s="3">
+      <c r="E26" s="3">
         <v>0.27088983565410402</v>
       </c>
-      <c r="E26" s="9">
+      <c r="F26" s="9">
         <f>SUM(Table1[[#This Row],[red leaves, temple and shrines]:[leisure activities]])</f>
         <v>1.0177092719825671</v>
       </c>
     </row>
-    <row r="27" spans="1:5">
-      <c r="A27" s="1" t="s">
+    <row r="27" spans="2:6">
+      <c r="B27" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="B27" s="2">
+      <c r="C27" s="2">
         <v>0.54885801506965604</v>
       </c>
-      <c r="C27">
+      <c r="D27">
         <v>0.17606836507155399</v>
       </c>
-      <c r="D27" s="3">
+      <c r="E27" s="3">
         <v>0.280253857175909</v>
       </c>
-      <c r="E27" s="9">
+      <c r="F27" s="9">
         <f>SUM(Table1[[#This Row],[red leaves, temple and shrines]:[leisure activities]])</f>
         <v>1.005180237317119</v>
       </c>
     </row>
-    <row r="28" spans="1:5">
-      <c r="A28" s="1" t="s">
+    <row r="28" spans="2:6">
+      <c r="B28" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="B28" s="2">
+      <c r="C28" s="2">
         <v>0.37002545176833201</v>
       </c>
-      <c r="C28">
+      <c r="D28">
         <v>0.30259155065307602</v>
       </c>
-      <c r="D28" s="3">
+      <c r="E28" s="3">
         <v>0.33085725393520099</v>
       </c>
-      <c r="E28" s="9">
+      <c r="F28" s="9">
         <f>SUM(Table1[[#This Row],[red leaves, temple and shrines]:[leisure activities]])</f>
         <v>1.003474256356609</v>
       </c>
     </row>
-    <row r="29" spans="1:5">
-      <c r="A29" s="1" t="s">
+    <row r="29" spans="2:6">
+      <c r="B29" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="B29" s="2">
+      <c r="C29" s="2">
         <v>0.54901529759286505</v>
       </c>
-      <c r="C29">
+      <c r="D29">
         <v>0.287155135257879</v>
       </c>
-      <c r="D29" s="3">
+      <c r="E29" s="3">
         <v>0.12535601227357501</v>
       </c>
-      <c r="E29" s="9">
+      <c r="F29" s="9">
         <f>SUM(Table1[[#This Row],[red leaves, temple and shrines]:[leisure activities]])</f>
         <v>0.96152644512431906</v>
       </c>
     </row>
-    <row r="30" spans="1:5">
-      <c r="A30" s="1" t="s">
+    <row r="30" spans="2:6">
+      <c r="B30" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="B30" s="2">
+      <c r="C30" s="2">
         <v>0.74786406251777704</v>
       </c>
-      <c r="C30">
+      <c r="D30">
         <v>2.4466139546941199E-2</v>
       </c>
-      <c r="D30" s="3">
+      <c r="E30" s="3">
         <v>0.12535601227357501</v>
       </c>
-      <c r="E30" s="9">
+      <c r="F30" s="9">
         <f>SUM(Table1[[#This Row],[red leaves, temple and shrines]:[leisure activities]])</f>
         <v>0.89768621433829332</v>
       </c>
     </row>
-    <row r="31" spans="1:5">
-      <c r="A31" s="1" t="s">
+    <row r="31" spans="2:6">
+      <c r="B31" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="B31" s="2">
+      <c r="C31" s="2">
         <v>9.7541613744420802E-2</v>
       </c>
-      <c r="C31">
+      <c r="D31">
         <v>0.35772645010591703</v>
       </c>
-      <c r="D31" s="3">
+      <c r="E31" s="3">
         <v>0.28749173891801499</v>
       </c>
-      <c r="E31" s="9">
+      <c r="F31" s="9">
         <f>SUM(Table1[[#This Row],[red leaves, temple and shrines]:[leisure activities]])</f>
         <v>0.74275980276835285</v>
       </c>
     </row>
-    <row r="32" spans="1:5">
-      <c r="A32" s="1" t="s">
+    <row r="32" spans="2:6">
+      <c r="B32" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="B32" s="2">
+      <c r="C32" s="2">
         <v>0.37988430104084903</v>
       </c>
-      <c r="C32">
+      <c r="D32">
         <v>0.164487993682887</v>
       </c>
-      <c r="D32" s="3">
+      <c r="E32" s="3">
         <v>0.162020295483566</v>
       </c>
-      <c r="E32" s="9">
+      <c r="F32" s="9">
         <f>SUM(Table1[[#This Row],[red leaves, temple and shrines]:[leisure activities]])</f>
         <v>0.70639259020730205</v>
       </c>
     </row>
-    <row r="33" spans="1:5">
-      <c r="A33" s="1" t="s">
+    <row r="33" spans="2:7">
+      <c r="B33" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="B33" s="2">
+      <c r="C33" s="2">
         <v>0.44714418753246998</v>
       </c>
-      <c r="C33">
+      <c r="D33">
         <v>0.12652318558152101</v>
       </c>
-      <c r="D33" s="3">
+      <c r="E33" s="3">
         <v>9.93422893467788E-2</v>
       </c>
-      <c r="E33" s="9">
+      <c r="F33" s="9">
         <f>SUM(Table1[[#This Row],[red leaves, temple and shrines]:[leisure activities]])</f>
         <v>0.67300966246076976</v>
       </c>
     </row>
-    <row r="34" spans="1:5">
-      <c r="A34" s="1" t="s">
+    <row r="34" spans="2:7">
+      <c r="B34" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="B34" s="2">
+      <c r="C34" s="2">
         <v>0.29561788291983199</v>
       </c>
-      <c r="C34">
+      <c r="D34">
         <v>0.19150478046675101</v>
       </c>
-      <c r="D34" s="3">
+      <c r="E34" s="3">
         <v>0.18091156782913001</v>
       </c>
-      <c r="E34" s="9">
+      <c r="F34" s="9">
         <f>SUM(Table1[[#This Row],[red leaves, temple and shrines]:[leisure activities]])</f>
         <v>0.66803423121571304</v>
       </c>
     </row>
-    <row r="35" spans="1:5">
-      <c r="A35" s="1" t="s">
+    <row r="35" spans="2:7">
+      <c r="B35" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="B35" s="2">
+      <c r="C35" s="2">
         <v>0.39346805907529397</v>
       </c>
-      <c r="C35">
+      <c r="D35">
         <v>0.111086770186325</v>
       </c>
-      <c r="D35" s="3">
+      <c r="E35" s="3">
         <v>0.12535601227357501</v>
       </c>
-      <c r="E35" s="9">
+      <c r="F35" s="9">
         <f>SUM(Table1[[#This Row],[red leaves, temple and shrines]:[leisure activities]])</f>
         <v>0.62991084153519394</v>
       </c>
     </row>
-    <row r="36" spans="1:5">
-      <c r="A36" s="1" t="s">
+    <row r="36" spans="2:7">
+      <c r="B36" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="B36" s="2">
+      <c r="C36" s="2">
         <v>0.45060522810819598</v>
       </c>
-      <c r="C36">
+      <c r="D36">
         <v>1.54364153951964E-2</v>
       </c>
-      <c r="D36" s="3">
+      <c r="E36" s="3">
         <v>0.145533823380529</v>
       </c>
-      <c r="E36" s="9">
+      <c r="F36" s="9">
         <f>SUM(Table1[[#This Row],[red leaves, temple and shrines]:[leisure activities]])</f>
         <v>0.61157546688392139</v>
       </c>
     </row>
-    <row r="37" spans="1:5">
-      <c r="A37" s="1" t="s">
+    <row r="37" spans="2:7">
+      <c r="B37" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="B37" s="2">
+      <c r="C37" s="2">
         <v>0.30166363081053499</v>
       </c>
-      <c r="C37">
+      <c r="D37">
         <v>0</v>
       </c>
-      <c r="D37" s="3">
+      <c r="E37" s="3">
         <v>0</v>
       </c>
-      <c r="E37" s="9">
+      <c r="F37" s="9">
         <f>SUM(Table1[[#This Row],[red leaves, temple and shrines]:[leisure activities]])</f>
         <v>0.30166363081053499</v>
       </c>
     </row>
-    <row r="38" spans="1:5">
-      <c r="A38" s="1" t="s">
+    <row r="38" spans="2:7">
+      <c r="B38" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="B38" s="2">
+      <c r="C38" s="2">
         <v>0</v>
       </c>
-      <c r="C38">
+      <c r="D38">
         <v>0</v>
       </c>
-      <c r="D38" s="3">
+      <c r="E38" s="3">
         <v>6.2678006136787506E-2</v>
       </c>
-      <c r="E38" s="9">
+      <c r="F38" s="9">
         <f>SUM(Table1[[#This Row],[red leaves, temple and shrines]:[leisure activities]])</f>
         <v>6.2678006136787506E-2</v>
       </c>
     </row>
+    <row r="43" spans="2:7">
+      <c r="C43">
+        <v>1</v>
+      </c>
+      <c r="D43" t="s">
+        <v>1</v>
+      </c>
+      <c r="F43">
+        <v>24</v>
+      </c>
+      <c r="G43" s="19" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="44" spans="2:7" ht="30">
+      <c r="C44">
+        <v>2</v>
+      </c>
+      <c r="D44" t="s">
+        <v>2</v>
+      </c>
+      <c r="F44">
+        <v>17</v>
+      </c>
+      <c r="G44" s="20" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="45" spans="2:7" ht="30">
+      <c r="C45">
+        <v>3</v>
+      </c>
+      <c r="D45" t="s">
+        <v>3</v>
+      </c>
+      <c r="F45">
+        <v>25</v>
+      </c>
+      <c r="G45" s="19" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="46" spans="2:7">
+      <c r="C46">
+        <v>4</v>
+      </c>
+      <c r="D46" t="s">
+        <v>4</v>
+      </c>
+      <c r="F46">
+        <v>23</v>
+      </c>
+      <c r="G46" s="20" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="47" spans="2:7">
+      <c r="C47">
+        <v>5</v>
+      </c>
+      <c r="D47" t="s">
+        <v>5</v>
+      </c>
+      <c r="F47">
+        <v>29</v>
+      </c>
+      <c r="G47" s="19" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="48" spans="2:7" ht="30">
+      <c r="C48">
+        <v>6</v>
+      </c>
+      <c r="D48" t="s">
+        <v>6</v>
+      </c>
+      <c r="F48">
+        <v>13</v>
+      </c>
+      <c r="G48" s="20" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="49" spans="3:7">
+      <c r="C49">
+        <v>7</v>
+      </c>
+      <c r="D49" t="s">
+        <v>7</v>
+      </c>
+      <c r="F49">
+        <v>14</v>
+      </c>
+      <c r="G49" s="19" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="50" spans="3:7" ht="30">
+      <c r="C50">
+        <v>8</v>
+      </c>
+      <c r="D50" t="s">
+        <v>8</v>
+      </c>
+      <c r="F50">
+        <v>16</v>
+      </c>
+      <c r="G50" s="20" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="51" spans="3:7" ht="30">
+      <c r="C51">
+        <v>9</v>
+      </c>
+      <c r="D51" t="s">
+        <v>9</v>
+      </c>
+      <c r="F51">
+        <v>1</v>
+      </c>
+      <c r="G51" s="19" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="52" spans="3:7">
+      <c r="C52">
+        <v>10</v>
+      </c>
+      <c r="D52" t="s">
+        <v>10</v>
+      </c>
+      <c r="F52">
+        <v>27</v>
+      </c>
+      <c r="G52" s="20" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="53" spans="3:7" ht="30">
+      <c r="C53">
+        <v>11</v>
+      </c>
+      <c r="D53" t="s">
+        <v>11</v>
+      </c>
+      <c r="F53">
+        <v>12</v>
+      </c>
+      <c r="G53" s="19" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="54" spans="3:7" ht="30">
+      <c r="C54">
+        <v>12</v>
+      </c>
+      <c r="D54" t="s">
+        <v>12</v>
+      </c>
+      <c r="F54">
+        <v>11</v>
+      </c>
+      <c r="G54" s="20" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="55" spans="3:7">
+      <c r="C55">
+        <v>13</v>
+      </c>
+      <c r="D55" t="s">
+        <v>13</v>
+      </c>
+      <c r="F55">
+        <v>3</v>
+      </c>
+      <c r="G55" s="19" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="56" spans="3:7">
+      <c r="C56">
+        <v>14</v>
+      </c>
+      <c r="D56" t="s">
+        <v>14</v>
+      </c>
+      <c r="F56">
+        <v>36</v>
+      </c>
+      <c r="G56" s="20" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="57" spans="3:7" ht="30">
+      <c r="C57">
+        <v>15</v>
+      </c>
+      <c r="D57" t="s">
+        <v>15</v>
+      </c>
+      <c r="F57">
+        <v>33</v>
+      </c>
+      <c r="G57" s="19" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="58" spans="3:7">
+      <c r="C58">
+        <v>16</v>
+      </c>
+      <c r="D58" t="s">
+        <v>16</v>
+      </c>
+      <c r="F58">
+        <v>20</v>
+      </c>
+      <c r="G58" s="20" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="59" spans="3:7">
+      <c r="C59">
+        <v>17</v>
+      </c>
+      <c r="D59" t="s">
+        <v>17</v>
+      </c>
+      <c r="F59">
+        <v>21</v>
+      </c>
+      <c r="G59" s="19" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="60" spans="3:7" ht="30">
+      <c r="C60">
+        <v>18</v>
+      </c>
+      <c r="D60" t="s">
+        <v>18</v>
+      </c>
+      <c r="F60">
+        <v>28</v>
+      </c>
+      <c r="G60" s="20" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="61" spans="3:7">
+      <c r="C61">
+        <v>19</v>
+      </c>
+      <c r="D61" t="s">
+        <v>19</v>
+      </c>
+      <c r="F61">
+        <v>31</v>
+      </c>
+      <c r="G61" s="19" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="62" spans="3:7">
+      <c r="C62">
+        <v>20</v>
+      </c>
+      <c r="D62" t="s">
+        <v>20</v>
+      </c>
+      <c r="F62">
+        <v>2</v>
+      </c>
+      <c r="G62" s="20" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="63" spans="3:7">
+      <c r="C63">
+        <v>21</v>
+      </c>
+      <c r="D63" t="s">
+        <v>21</v>
+      </c>
+      <c r="F63">
+        <v>19</v>
+      </c>
+      <c r="G63" s="19" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="64" spans="3:7">
+      <c r="C64">
+        <v>22</v>
+      </c>
+      <c r="D64" t="s">
+        <v>22</v>
+      </c>
+      <c r="F64">
+        <v>10</v>
+      </c>
+      <c r="G64" s="20" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="65" spans="3:7">
+      <c r="C65">
+        <v>23</v>
+      </c>
+      <c r="D65" t="s">
+        <v>23</v>
+      </c>
+      <c r="F65">
+        <v>32</v>
+      </c>
+      <c r="G65" s="19" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="66" spans="3:7" ht="30">
+      <c r="C66">
+        <v>24</v>
+      </c>
+      <c r="D66" t="s">
+        <v>24</v>
+      </c>
+      <c r="F66">
+        <v>26</v>
+      </c>
+      <c r="G66" s="20" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="67" spans="3:7">
+      <c r="C67">
+        <v>25</v>
+      </c>
+      <c r="D67" t="s">
+        <v>25</v>
+      </c>
+      <c r="F67">
+        <v>9</v>
+      </c>
+      <c r="G67" s="19" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="68" spans="3:7">
+      <c r="C68">
+        <v>26</v>
+      </c>
+      <c r="D68" t="s">
+        <v>26</v>
+      </c>
+      <c r="F68">
+        <v>34</v>
+      </c>
+      <c r="G68" s="20" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="69" spans="3:7" ht="30">
+      <c r="C69">
+        <v>27</v>
+      </c>
+      <c r="D69" t="s">
+        <v>27</v>
+      </c>
+      <c r="F69">
+        <v>4</v>
+      </c>
+      <c r="G69" s="19" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="70" spans="3:7">
+      <c r="C70">
+        <v>28</v>
+      </c>
+      <c r="D70" t="s">
+        <v>28</v>
+      </c>
+      <c r="F70">
+        <v>5</v>
+      </c>
+      <c r="G70" s="20" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="71" spans="3:7" ht="30">
+      <c r="C71">
+        <v>29</v>
+      </c>
+      <c r="D71" t="s">
+        <v>29</v>
+      </c>
+      <c r="F71">
+        <v>6</v>
+      </c>
+      <c r="G71" s="19" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="72" spans="3:7">
+      <c r="C72">
+        <v>30</v>
+      </c>
+      <c r="D72" t="s">
+        <v>30</v>
+      </c>
+      <c r="F72">
+        <v>8</v>
+      </c>
+      <c r="G72" s="20" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="73" spans="3:7">
+      <c r="C73">
+        <v>31</v>
+      </c>
+      <c r="D73" t="s">
+        <v>31</v>
+      </c>
+      <c r="F73">
+        <v>18</v>
+      </c>
+      <c r="G73" s="19" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="74" spans="3:7">
+      <c r="C74">
+        <v>32</v>
+      </c>
+      <c r="D74" t="s">
+        <v>32</v>
+      </c>
+      <c r="F74">
+        <v>15</v>
+      </c>
+      <c r="G74" s="20" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="75" spans="3:7">
+      <c r="C75">
+        <v>33</v>
+      </c>
+      <c r="D75" t="s">
+        <v>33</v>
+      </c>
+      <c r="F75">
+        <v>22</v>
+      </c>
+      <c r="G75" s="19" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="76" spans="3:7">
+      <c r="C76">
+        <v>34</v>
+      </c>
+      <c r="D76" t="s">
+        <v>34</v>
+      </c>
+      <c r="F76">
+        <v>35</v>
+      </c>
+      <c r="G76" s="20" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="77" spans="3:7">
+      <c r="C77">
+        <v>35</v>
+      </c>
+      <c r="D77" t="s">
+        <v>35</v>
+      </c>
+      <c r="F77">
+        <v>7</v>
+      </c>
+      <c r="G77" s="19" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="78" spans="3:7">
+      <c r="C78">
+        <v>36</v>
+      </c>
+      <c r="D78" t="s">
+        <v>36</v>
+      </c>
+      <c r="F78">
+        <v>37</v>
+      </c>
+      <c r="G78" s="20" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="79" spans="3:7">
+      <c r="C79">
+        <v>37</v>
+      </c>
+      <c r="D79" t="s">
+        <v>37</v>
+      </c>
+      <c r="F79">
+        <v>30</v>
+      </c>
+      <c r="G79" s="19" t="s">
+        <v>30</v>
+      </c>
+    </row>
   </sheetData>
   <mergeCells count="20">
-    <mergeCell ref="Q9:R9"/>
-    <mergeCell ref="S9:T9"/>
-    <mergeCell ref="Q10:R10"/>
-    <mergeCell ref="S10:T10"/>
-    <mergeCell ref="Q11:R11"/>
-    <mergeCell ref="S11:T11"/>
-    <mergeCell ref="Q6:R6"/>
-    <mergeCell ref="S6:T6"/>
-    <mergeCell ref="Q7:R7"/>
-    <mergeCell ref="S7:T7"/>
-    <mergeCell ref="Q8:R8"/>
-    <mergeCell ref="S8:T8"/>
-    <mergeCell ref="Q5:R5"/>
-    <mergeCell ref="S5:T5"/>
-    <mergeCell ref="Q2:R2"/>
-    <mergeCell ref="S2:T2"/>
-    <mergeCell ref="Q3:R3"/>
-    <mergeCell ref="S3:T3"/>
-    <mergeCell ref="Q4:R4"/>
-    <mergeCell ref="S4:T4"/>
+    <mergeCell ref="R5:S5"/>
+    <mergeCell ref="T5:U5"/>
+    <mergeCell ref="R2:S2"/>
+    <mergeCell ref="T2:U2"/>
+    <mergeCell ref="R3:S3"/>
+    <mergeCell ref="T3:U3"/>
+    <mergeCell ref="R4:S4"/>
+    <mergeCell ref="T4:U4"/>
+    <mergeCell ref="R6:S6"/>
+    <mergeCell ref="T6:U6"/>
+    <mergeCell ref="R7:S7"/>
+    <mergeCell ref="T7:U7"/>
+    <mergeCell ref="R8:S8"/>
+    <mergeCell ref="T8:U8"/>
+    <mergeCell ref="R9:S9"/>
+    <mergeCell ref="T9:U9"/>
+    <mergeCell ref="R10:S10"/>
+    <mergeCell ref="T10:U10"/>
+    <mergeCell ref="R11:S11"/>
+    <mergeCell ref="T11:U11"/>
   </mergeCells>
-  <conditionalFormatting sqref="B2:D38">
+  <conditionalFormatting sqref="C2:E38">
     <cfRule type="colorScale" priority="2">
       <colorScale>
         <cfvo type="min"/>
@@ -4348,7 +4847,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E2:E38">
+  <conditionalFormatting sqref="F2:F38">
     <cfRule type="colorScale" priority="1">
       <colorScale>
         <cfvo type="min"/>
@@ -4368,700 +4867,1121 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A9A4F8E8-4F1F-4C47-9C71-074BFF072A3E}">
-  <dimension ref="A1:E38"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BE540D85-721F-BC40-8120-CC81BEC4477C}">
+  <dimension ref="B1:C38"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A9" workbookViewId="0">
-      <selection activeCell="F4" sqref="F4"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B1" sqref="B1:C38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
+  <cols>
+    <col min="2" max="2" width="10.6640625" customWidth="1"/>
+    <col min="3" max="3" width="19.33203125" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:5">
+    <row r="1" spans="2:3">
+      <c r="B1" t="s">
+        <v>63</v>
+      </c>
+      <c r="C1" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="2" spans="2:3">
+      <c r="B2">
+        <v>1</v>
+      </c>
+      <c r="C2" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="2:3">
+      <c r="B3">
+        <v>2</v>
+      </c>
+      <c r="C3" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4" spans="2:3">
+      <c r="B4">
+        <v>3</v>
+      </c>
+      <c r="C4" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="5" spans="2:3">
+      <c r="B5">
+        <v>4</v>
+      </c>
+      <c r="C5" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="6" spans="2:3">
+      <c r="B6">
+        <v>5</v>
+      </c>
+      <c r="C6" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="7" spans="2:3">
+      <c r="B7">
+        <v>6</v>
+      </c>
+      <c r="C7" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="8" spans="2:3">
+      <c r="B8">
+        <v>7</v>
+      </c>
+      <c r="C8" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="9" spans="2:3">
+      <c r="B9">
+        <v>8</v>
+      </c>
+      <c r="C9" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="10" spans="2:3">
+      <c r="B10">
+        <v>9</v>
+      </c>
+      <c r="C10" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="11" spans="2:3">
+      <c r="B11">
+        <v>10</v>
+      </c>
+      <c r="C11" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="12" spans="2:3">
+      <c r="B12">
+        <v>11</v>
+      </c>
+      <c r="C12" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="13" spans="2:3">
+      <c r="B13">
+        <v>12</v>
+      </c>
+      <c r="C13" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="14" spans="2:3">
+      <c r="B14">
+        <v>13</v>
+      </c>
+      <c r="C14" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="15" spans="2:3">
+      <c r="B15">
+        <v>14</v>
+      </c>
+      <c r="C15" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="16" spans="2:3">
+      <c r="B16">
+        <v>15</v>
+      </c>
+      <c r="C16" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="17" spans="2:3">
+      <c r="B17">
+        <v>16</v>
+      </c>
+      <c r="C17" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="18" spans="2:3">
+      <c r="B18">
+        <v>17</v>
+      </c>
+      <c r="C18" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="19" spans="2:3">
+      <c r="B19">
+        <v>18</v>
+      </c>
+      <c r="C19" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="20" spans="2:3">
+      <c r="B20">
+        <v>19</v>
+      </c>
+      <c r="C20" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="21" spans="2:3">
+      <c r="B21">
+        <v>20</v>
+      </c>
+      <c r="C21" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="22" spans="2:3">
+      <c r="B22">
+        <v>21</v>
+      </c>
+      <c r="C22" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="23" spans="2:3">
+      <c r="B23">
+        <v>22</v>
+      </c>
+      <c r="C23" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="24" spans="2:3">
+      <c r="B24">
+        <v>23</v>
+      </c>
+      <c r="C24" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="25" spans="2:3">
+      <c r="B25">
+        <v>24</v>
+      </c>
+      <c r="C25" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="26" spans="2:3">
+      <c r="B26">
+        <v>25</v>
+      </c>
+      <c r="C26" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="27" spans="2:3">
+      <c r="B27">
+        <v>26</v>
+      </c>
+      <c r="C27" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="28" spans="2:3">
+      <c r="B28">
+        <v>27</v>
+      </c>
+      <c r="C28" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="29" spans="2:3">
+      <c r="B29">
+        <v>28</v>
+      </c>
+      <c r="C29" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="30" spans="2:3">
+      <c r="B30">
+        <v>29</v>
+      </c>
+      <c r="C30" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="31" spans="2:3">
+      <c r="B31">
+        <v>30</v>
+      </c>
+      <c r="C31" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="32" spans="2:3">
+      <c r="B32">
+        <v>31</v>
+      </c>
+      <c r="C32" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="33" spans="2:3">
+      <c r="B33">
+        <v>32</v>
+      </c>
+      <c r="C33" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="34" spans="2:3">
+      <c r="B34">
+        <v>33</v>
+      </c>
+      <c r="C34" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="35" spans="2:3">
+      <c r="B35">
+        <v>34</v>
+      </c>
+      <c r="C35" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="36" spans="2:3">
+      <c r="B36">
+        <v>35</v>
+      </c>
+      <c r="C36" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="37" spans="2:3">
+      <c r="B37">
+        <v>36</v>
+      </c>
+      <c r="C37" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="38" spans="2:3">
+      <c r="B38">
+        <v>37</v>
+      </c>
+      <c r="C38" t="s">
+        <v>37</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <tableParts count="1">
+    <tablePart r:id="rId1"/>
+  </tableParts>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6FA42994-71E1-E54B-A37F-1E4545E2FB02}">
+  <dimension ref="A1:F38"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B12" sqref="B12"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
+  <cols>
+    <col min="1" max="1" width="12.5" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="19.33203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.5" customWidth="1"/>
+    <col min="4" max="4" width="12.1640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12.6640625" customWidth="1"/>
+    <col min="6" max="6" width="12.1640625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6">
       <c r="A1" t="s">
+        <v>62</v>
+      </c>
+      <c r="B1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C1" t="s">
         <v>60</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>61</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>50</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="2" spans="1:5">
-      <c r="A2" s="1" t="s">
+    <row r="2" spans="1:6">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C2">
+        <v>0.84559953924055298</v>
+      </c>
+      <c r="D2">
+        <v>0.311859991058062</v>
+      </c>
+      <c r="E2">
+        <v>0.39136496828702</v>
+      </c>
+      <c r="F2">
+        <v>1.548824498585635</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="B3" t="s">
+        <v>2</v>
+      </c>
+      <c r="C3">
+        <v>0.51750653091780496</v>
+      </c>
+      <c r="D3">
+        <v>0.36413314134936797</v>
+      </c>
+      <c r="E3">
+        <v>0.26376738507287201</v>
+      </c>
+      <c r="F3">
+        <v>1.1454070573400448</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6">
+      <c r="A4">
+        <v>3</v>
+      </c>
+      <c r="B4" t="s">
+        <v>3</v>
+      </c>
+      <c r="C4">
+        <v>0.44372111837551997</v>
+      </c>
+      <c r="D4">
+        <v>0.38300956093350202</v>
+      </c>
+      <c r="E4">
+        <v>0.48815989908006302</v>
+      </c>
+      <c r="F4">
+        <v>1.314890578389085</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6">
+      <c r="A5">
+        <v>4</v>
+      </c>
+      <c r="B5" t="s">
+        <v>4</v>
+      </c>
+      <c r="C5">
+        <v>0.37002545176833201</v>
+      </c>
+      <c r="D5">
+        <v>0.30259155065307602</v>
+      </c>
+      <c r="E5">
+        <v>0.33085725393520099</v>
+      </c>
+      <c r="F5">
+        <v>1.003474256356609</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6">
+      <c r="A6">
+        <v>5</v>
+      </c>
+      <c r="B6" t="s">
+        <v>5</v>
+      </c>
+      <c r="C6">
+        <v>0.54901529759286505</v>
+      </c>
+      <c r="D6">
+        <v>0.287155135257879</v>
+      </c>
+      <c r="E6">
+        <v>0.12535601227357501</v>
+      </c>
+      <c r="F6">
+        <v>0.96152644512431906</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6">
+      <c r="A7">
+        <v>6</v>
+      </c>
+      <c r="B7" t="s">
+        <v>6</v>
+      </c>
+      <c r="C7">
+        <v>0.74786406251777704</v>
+      </c>
+      <c r="D7">
+        <v>2.4466139546941199E-2</v>
+      </c>
+      <c r="E7">
+        <v>0.12535601227357501</v>
+      </c>
+      <c r="F7">
+        <v>0.89768621433829332</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6">
+      <c r="A8">
+        <v>7</v>
+      </c>
+      <c r="B8" t="s">
+        <v>7</v>
+      </c>
+      <c r="C8">
+        <v>0.45060522810819598</v>
+      </c>
+      <c r="D8">
+        <v>1.54364153951964E-2</v>
+      </c>
+      <c r="E8">
+        <v>0.145533823380529</v>
+      </c>
+      <c r="F8">
+        <v>0.61157546688392139</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6">
+      <c r="A9">
+        <v>8</v>
+      </c>
+      <c r="B9" t="s">
+        <v>8</v>
+      </c>
+      <c r="C9">
+        <v>9.7541613744420802E-2</v>
+      </c>
+      <c r="D9">
+        <v>0.35772645010591703</v>
+      </c>
+      <c r="E9">
+        <v>0.28749173891801499</v>
+      </c>
+      <c r="F9">
+        <v>0.74275980276835285</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6">
+      <c r="A10">
+        <v>9</v>
+      </c>
+      <c r="B10" t="s">
+        <v>9</v>
+      </c>
+      <c r="C10">
+        <v>0.37021656663841301</v>
+      </c>
+      <c r="D10">
+        <v>0.37660286969005002</v>
+      </c>
+      <c r="E10">
+        <v>0.27088983565410402</v>
+      </c>
+      <c r="F10">
+        <v>1.0177092719825671</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6">
+      <c r="A11">
+        <v>10</v>
+      </c>
+      <c r="B11" t="s">
+        <v>10</v>
+      </c>
+      <c r="C11">
+        <v>0.531498341761096</v>
+      </c>
+      <c r="D11">
+        <v>0.287155135257879</v>
+      </c>
+      <c r="E11">
+        <v>0.30131542130644201</v>
+      </c>
+      <c r="F11">
+        <v>1.119968898325417</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6">
+      <c r="A12">
+        <v>11</v>
+      </c>
+      <c r="B12" t="s">
+        <v>11</v>
+      </c>
+      <c r="C12">
+        <v>0.55196481794434304</v>
+      </c>
+      <c r="D12">
+        <v>0.46284931618652497</v>
+      </c>
+      <c r="E12">
+        <v>0.31691814038589999</v>
+      </c>
+      <c r="F12">
+        <v>1.3317322745167681</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6">
+      <c r="A13">
+        <v>12</v>
+      </c>
+      <c r="B13" t="s">
+        <v>12</v>
+      </c>
+      <c r="C13">
+        <v>0.49709465907878803</v>
+      </c>
+      <c r="D13">
+        <v>0.58630668172201905</v>
+      </c>
+      <c r="E13">
+        <v>0.321493232413396</v>
+      </c>
+      <c r="F13">
+        <v>1.4048945732142029</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6">
+      <c r="A14">
+        <v>13</v>
+      </c>
+      <c r="B14" t="s">
+        <v>13</v>
+      </c>
+      <c r="C14">
+        <v>0.647873331891062</v>
+      </c>
+      <c r="D14">
+        <v>0.58974668591095603</v>
+      </c>
+      <c r="E14">
+        <v>0.61134561956866995</v>
+      </c>
+      <c r="F14">
+        <v>1.848965637370688</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6">
+      <c r="A15">
+        <v>14</v>
+      </c>
+      <c r="B15" t="s">
+        <v>14</v>
+      </c>
+      <c r="C15">
+        <v>0.86517596384200002</v>
+      </c>
+      <c r="D15">
+        <v>0.44741290079132801</v>
+      </c>
+      <c r="E15">
+        <v>0.36182313565826102</v>
+      </c>
+      <c r="F15">
+        <v>1.674412000291589</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6">
+      <c r="A16">
+        <v>15</v>
+      </c>
+      <c r="B16" t="s">
+        <v>15</v>
+      </c>
+      <c r="C16">
+        <v>0.44714418753246998</v>
+      </c>
+      <c r="D16">
+        <v>0.12652318558152101</v>
+      </c>
+      <c r="E16">
+        <v>9.93422893467788E-2</v>
+      </c>
+      <c r="F16">
+        <v>0.67300966246076976</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6">
+      <c r="A17">
+        <v>16</v>
+      </c>
+      <c r="B17" t="s">
+        <v>16</v>
+      </c>
+      <c r="C17">
+        <v>0.84804120995904297</v>
+      </c>
+      <c r="D17">
+        <v>0.42419964013700601</v>
+      </c>
+      <c r="E17">
+        <v>0.31932294062842798</v>
+      </c>
+      <c r="F17">
+        <v>1.5915637907244768</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6">
+      <c r="A18">
+        <v>17</v>
+      </c>
+      <c r="B18" t="s">
+        <v>17</v>
+      </c>
+      <c r="C18">
+        <v>0.69480038130807198</v>
+      </c>
+      <c r="D18">
+        <v>0.63404031916133596</v>
+      </c>
+      <c r="E18">
+        <v>0.79998075483900299</v>
+      </c>
+      <c r="F18">
+        <v>2.1288214553084108</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6">
+      <c r="A19">
+        <v>18</v>
+      </c>
+      <c r="B19" t="s">
+        <v>18</v>
+      </c>
+      <c r="C19">
+        <v>0.37988430104084903</v>
+      </c>
+      <c r="D19">
+        <v>0.164487993682887</v>
+      </c>
+      <c r="E19">
+        <v>0.162020295483566</v>
+      </c>
+      <c r="F19">
+        <v>0.70639259020730205</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6">
+      <c r="A20">
+        <v>19</v>
+      </c>
+      <c r="B20" t="s">
+        <v>19</v>
+      </c>
+      <c r="C20">
+        <v>0.45841234955560201</v>
+      </c>
+      <c r="D20">
+        <v>0.42294676124438702</v>
+      </c>
+      <c r="E20">
+        <v>0.256194021047779</v>
+      </c>
+      <c r="F20">
+        <v>1.1375531318477679</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6">
+      <c r="A21">
+        <v>20</v>
+      </c>
+      <c r="B21" t="s">
+        <v>21</v>
+      </c>
+      <c r="C21">
+        <v>0.30180992114149102</v>
+      </c>
+      <c r="D21">
+        <v>0.51239449567655704</v>
+      </c>
+      <c r="E21">
+        <v>0.37959614652268803</v>
+      </c>
+      <c r="F21">
+        <v>1.193800563340736</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6">
+      <c r="A22">
+        <v>21</v>
+      </c>
+      <c r="B22" t="s">
+        <v>20</v>
+      </c>
+      <c r="C22">
+        <v>0.387879268590961</v>
+      </c>
+      <c r="D22">
+        <v>0.48768257748393101</v>
+      </c>
+      <c r="E22">
+        <v>0.31691814038589999</v>
+      </c>
+      <c r="F22">
+        <v>1.192479986460792</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6">
+      <c r="A23">
+        <v>22</v>
+      </c>
+      <c r="B23" t="s">
+        <v>22</v>
+      </c>
+      <c r="C23">
+        <v>0.29561788291983199</v>
+      </c>
+      <c r="D23">
+        <v>0.19150478046675101</v>
+      </c>
+      <c r="E23">
+        <v>0.18091156782913001</v>
+      </c>
+      <c r="F23">
+        <v>0.66803423121571304</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6">
+      <c r="A24">
+        <v>23</v>
+      </c>
+      <c r="B24" t="s">
+        <v>23</v>
+      </c>
+      <c r="C24">
+        <v>0.75886464920609997</v>
+      </c>
+      <c r="D24">
+        <v>0.66597361433972002</v>
+      </c>
+      <c r="E24">
+        <v>0.46840330674714598</v>
+      </c>
+      <c r="F24">
+        <v>1.8932415702929661</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6">
+      <c r="A25">
         <v>24</v>
       </c>
-      <c r="B2" s="2">
+      <c r="B25" t="s">
+        <v>24</v>
+      </c>
+      <c r="C25">
         <v>0.76629066303512905</v>
       </c>
-      <c r="C2">
+      <c r="D25">
         <v>0.843982451523971</v>
       </c>
-      <c r="D2" s="3">
+      <c r="E25">
         <v>0.89736915738711498</v>
       </c>
-      <c r="E2" s="9">
-        <f>SUM(Table13[[#This Row],[red leaves, temple and shrines]:[leisure activities]])</f>
+      <c r="F25">
         <v>2.507642271946215</v>
       </c>
     </row>
-    <row r="3" spans="1:5" ht="30">
-      <c r="A3" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="B3" s="2">
-        <v>0.69480038130807198</v>
-      </c>
-      <c r="C3">
-        <v>0.63404031916133596</v>
-      </c>
-      <c r="D3" s="3">
-        <v>0.79998075483900299</v>
-      </c>
-      <c r="E3" s="9">
-        <f>SUM(Table13[[#This Row],[red leaves, temple and shrines]:[leisure activities]])</f>
-        <v>2.1288214553084108</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" ht="30">
-      <c r="A4" s="1" t="s">
+    <row r="26" spans="1:6">
+      <c r="A26">
         <v>25</v>
       </c>
-      <c r="B4" s="2">
+      <c r="B26" t="s">
+        <v>25</v>
+      </c>
+      <c r="C26">
         <v>0.38773301736600302</v>
       </c>
-      <c r="C4">
+      <c r="D26">
         <v>1</v>
       </c>
-      <c r="D4" s="3">
+      <c r="E26">
         <v>0.72222222222222199</v>
       </c>
-      <c r="E4" s="9">
-        <f>SUM(Table13[[#This Row],[red leaves, temple and shrines]:[leisure activities]])</f>
+      <c r="F26">
         <v>2.1099552395882251</v>
       </c>
     </row>
-    <row r="5" spans="1:5">
-      <c r="A5" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="B5" s="2">
-        <v>0.75886464920609997</v>
-      </c>
-      <c r="C5">
-        <v>0.66597361433972002</v>
-      </c>
-      <c r="D5" s="3">
-        <v>0.46840330674714598</v>
-      </c>
-      <c r="E5" s="9">
-        <f>SUM(Table13[[#This Row],[red leaves, temple and shrines]:[leisure activities]])</f>
-        <v>1.8932415702929661</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5">
-      <c r="A6" s="1" t="s">
+    <row r="27" spans="1:6">
+      <c r="A27">
+        <v>26</v>
+      </c>
+      <c r="B27" t="s">
+        <v>26</v>
+      </c>
+      <c r="C27">
+        <v>0.45363652525970799</v>
+      </c>
+      <c r="D27">
+        <v>0.33632613060500299</v>
+      </c>
+      <c r="E27">
+        <v>0.24358957396591799</v>
+      </c>
+      <c r="F27">
+        <v>1.033552229830629</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6">
+      <c r="A28">
+        <v>27</v>
+      </c>
+      <c r="B28" t="s">
+        <v>27</v>
+      </c>
+      <c r="C28">
+        <v>0.56018420706636796</v>
+      </c>
+      <c r="D28">
+        <v>0.464471120054052</v>
+      </c>
+      <c r="E28">
+        <v>0.412426532417553</v>
+      </c>
+      <c r="F28">
+        <v>1.4370818595379728</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6">
+      <c r="A29">
+        <v>28</v>
+      </c>
+      <c r="B29" t="s">
+        <v>28</v>
+      </c>
+      <c r="C29">
+        <v>0.42001622542966099</v>
+      </c>
+      <c r="D29">
+        <v>0.39348840239919097</v>
+      </c>
+      <c r="E29">
+        <v>0.36535124536022401</v>
+      </c>
+      <c r="F29">
+        <v>1.1788558731890761</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6">
+      <c r="A30">
         <v>29</v>
       </c>
-      <c r="B6" s="2">
+      <c r="B30" t="s">
+        <v>29</v>
+      </c>
+      <c r="C30">
         <v>0.49281036074163298</v>
       </c>
-      <c r="C6">
+      <c r="D30">
         <v>0.75070339259594698</v>
       </c>
-      <c r="D6" s="3">
+      <c r="E30">
         <v>0.61263215833006002</v>
       </c>
-      <c r="E6" s="9">
-        <f>SUM(Table13[[#This Row],[red leaves, temple and shrines]:[leisure activities]])</f>
+      <c r="F30">
         <v>1.85614591166764</v>
       </c>
     </row>
-    <row r="7" spans="1:5" ht="30">
-      <c r="A7" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="B7" s="2">
-        <v>0.647873331891062</v>
-      </c>
-      <c r="C7">
-        <v>0.58974668591095603</v>
-      </c>
-      <c r="D7" s="3">
-        <v>0.61134561956866995</v>
-      </c>
-      <c r="E7" s="9">
-        <f>SUM(Table13[[#This Row],[red leaves, temple and shrines]:[leisure activities]])</f>
-        <v>1.848965637370688</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5">
-      <c r="A8" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="B8" s="2">
-        <v>0.86517596384200002</v>
-      </c>
-      <c r="C8">
-        <v>0.44741290079132801</v>
-      </c>
-      <c r="D8" s="3">
-        <v>0.36182313565826102</v>
-      </c>
-      <c r="E8" s="9">
-        <f>SUM(Table13[[#This Row],[red leaves, temple and shrines]:[leisure activities]])</f>
-        <v>1.674412000291589</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" ht="30">
-      <c r="A9" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="B9" s="2">
-        <v>0.84804120995904297</v>
-      </c>
-      <c r="C9">
-        <v>0.42419964013700601</v>
-      </c>
-      <c r="D9" s="3">
-        <v>0.31932294062842798</v>
-      </c>
-      <c r="E9" s="9">
-        <f>SUM(Table13[[#This Row],[red leaves, temple and shrines]:[leisure activities]])</f>
-        <v>1.5915637907244768</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" ht="30">
-      <c r="A10" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="B10" s="2">
-        <v>0.84559953924055298</v>
-      </c>
-      <c r="C10">
-        <v>0.311859991058062</v>
-      </c>
-      <c r="D10" s="3">
-        <v>0.39136496828702</v>
-      </c>
-      <c r="E10" s="9">
-        <f>SUM(Table13[[#This Row],[red leaves, temple and shrines]:[leisure activities]])</f>
-        <v>1.548824498585635</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5">
-      <c r="A11" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="B11" s="2">
-        <v>0.56018420706636796</v>
-      </c>
-      <c r="C11">
-        <v>0.464471120054052</v>
-      </c>
-      <c r="D11" s="3">
-        <v>0.412426532417553</v>
-      </c>
-      <c r="E11" s="9">
-        <f>SUM(Table13[[#This Row],[red leaves, temple and shrines]:[leisure activities]])</f>
-        <v>1.4370818595379728</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5" ht="30">
-      <c r="A12" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="B12" s="2">
-        <v>0.49709465907878803</v>
-      </c>
-      <c r="C12">
-        <v>0.58630668172201905</v>
-      </c>
-      <c r="D12" s="3">
-        <v>0.321493232413396</v>
-      </c>
-      <c r="E12" s="9">
-        <f>SUM(Table13[[#This Row],[red leaves, temple and shrines]:[leisure activities]])</f>
-        <v>1.4048945732142029</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5" ht="30">
-      <c r="A13" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="B13" s="2">
-        <v>0.55196481794434304</v>
-      </c>
-      <c r="C13">
-        <v>0.46284931618652497</v>
-      </c>
-      <c r="D13" s="3">
-        <v>0.31691814038589999</v>
-      </c>
-      <c r="E13" s="9">
-        <f>SUM(Table13[[#This Row],[red leaves, temple and shrines]:[leisure activities]])</f>
-        <v>1.3317322745167681</v>
-      </c>
-    </row>
-    <row r="14" spans="1:5">
-      <c r="A14" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="B14" s="2">
-        <v>0.44372111837551997</v>
-      </c>
-      <c r="C14">
-        <v>0.38300956093350202</v>
-      </c>
-      <c r="D14" s="3">
-        <v>0.48815989908006302</v>
-      </c>
-      <c r="E14" s="9">
-        <f>SUM(Table13[[#This Row],[red leaves, temple and shrines]:[leisure activities]])</f>
-        <v>1.314890578389085</v>
-      </c>
-    </row>
-    <row r="15" spans="1:5">
-      <c r="A15" s="1" t="s">
+    <row r="31" spans="1:6">
+      <c r="A31">
+        <v>30</v>
+      </c>
+      <c r="B31" t="s">
+        <v>30</v>
+      </c>
+      <c r="C31">
+        <v>0</v>
+      </c>
+      <c r="D31">
+        <v>0</v>
+      </c>
+      <c r="E31">
+        <v>6.2678006136787506E-2</v>
+      </c>
+      <c r="F31">
+        <v>6.2678006136787506E-2</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6">
+      <c r="A32">
+        <v>31</v>
+      </c>
+      <c r="B32" t="s">
+        <v>31</v>
+      </c>
+      <c r="C32">
+        <v>0.59753013079116402</v>
+      </c>
+      <c r="D32">
+        <v>0.33326031055897498</v>
+      </c>
+      <c r="E32">
+        <v>0.22469830162035301</v>
+      </c>
+      <c r="F32">
+        <v>1.1554887429704921</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6">
+      <c r="A33">
+        <v>32</v>
+      </c>
+      <c r="B33" t="s">
+        <v>32</v>
+      </c>
+      <c r="C33">
+        <v>0.45001851657071301</v>
+      </c>
+      <c r="D33">
+        <v>0.32299738184833798</v>
+      </c>
+      <c r="E33">
+        <v>0.27088983565410402</v>
+      </c>
+      <c r="F33">
+        <v>1.043905734073155</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6">
+      <c r="A34">
+        <v>33</v>
+      </c>
+      <c r="B34" t="s">
+        <v>33</v>
+      </c>
+      <c r="C34">
+        <v>0.50735715650678304</v>
+      </c>
+      <c r="D34">
+        <v>0.39824190544420501</v>
+      </c>
+      <c r="E34">
+        <v>0.29802686804033601</v>
+      </c>
+      <c r="F34">
+        <v>1.2036259299913241</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6">
+      <c r="A35">
+        <v>34</v>
+      </c>
+      <c r="B35" t="s">
+        <v>34</v>
+      </c>
+      <c r="C35">
+        <v>0.54885801506965604</v>
+      </c>
+      <c r="D35">
+        <v>0.17606836507155399</v>
+      </c>
+      <c r="E35">
+        <v>0.280253857175909</v>
+      </c>
+      <c r="F35">
+        <v>1.005180237317119</v>
+      </c>
+    </row>
+    <row r="36" spans="1:6">
+      <c r="A36">
+        <v>35</v>
+      </c>
+      <c r="B36" t="s">
+        <v>35</v>
+      </c>
+      <c r="C36">
+        <v>0.39346805907529397</v>
+      </c>
+      <c r="D36">
+        <v>0.111086770186325</v>
+      </c>
+      <c r="E36">
+        <v>0.12535601227357501</v>
+      </c>
+      <c r="F36">
+        <v>0.62991084153519394</v>
+      </c>
+    </row>
+    <row r="37" spans="1:6">
+      <c r="A37">
         <v>36</v>
       </c>
-      <c r="B15" s="2">
+      <c r="B37" t="s">
+        <v>36</v>
+      </c>
+      <c r="C37">
         <v>0.21905617666692601</v>
       </c>
-      <c r="C15">
+      <c r="D37">
         <v>0.60518310130615205</v>
       </c>
-      <c r="D15" s="3">
+      <c r="E37">
         <v>0.38155003332135501</v>
       </c>
-      <c r="E15" s="9">
-        <f>SUM(Table13[[#This Row],[red leaves, temple and shrines]:[leisure activities]])</f>
+      <c r="F37">
         <v>1.2057893112944331</v>
       </c>
     </row>
-    <row r="16" spans="1:5" ht="30">
-      <c r="A16" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="B16" s="2">
-        <v>0.50735715650678304</v>
-      </c>
-      <c r="C16">
-        <v>0.39824190544420501</v>
-      </c>
-      <c r="D16" s="3">
-        <v>0.29802686804033601</v>
-      </c>
-      <c r="E16" s="9">
-        <f>SUM(Table13[[#This Row],[red leaves, temple and shrines]:[leisure activities]])</f>
-        <v>1.2036259299913241</v>
-      </c>
-    </row>
-    <row r="17" spans="1:5">
-      <c r="A17" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="B17" s="2">
-        <v>0.30180992114149102</v>
-      </c>
-      <c r="C17">
-        <v>0.51239449567655704</v>
-      </c>
-      <c r="D17" s="3">
-        <v>0.37959614652268803</v>
-      </c>
-      <c r="E17" s="9">
-        <f>SUM(Table13[[#This Row],[red leaves, temple and shrines]:[leisure activities]])</f>
-        <v>1.193800563340736</v>
-      </c>
-    </row>
-    <row r="18" spans="1:5">
-      <c r="A18" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="B18" s="2">
-        <v>0.387879268590961</v>
-      </c>
-      <c r="C18">
-        <v>0.48768257748393101</v>
-      </c>
-      <c r="D18" s="3">
-        <v>0.31691814038589999</v>
-      </c>
-      <c r="E18" s="9">
-        <f>SUM(Table13[[#This Row],[red leaves, temple and shrines]:[leisure activities]])</f>
-        <v>1.192479986460792</v>
-      </c>
-    </row>
-    <row r="19" spans="1:5" ht="30">
-      <c r="A19" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="B19" s="2">
-        <v>0.42001622542966099</v>
-      </c>
-      <c r="C19">
-        <v>0.39348840239919097</v>
-      </c>
-      <c r="D19" s="3">
-        <v>0.36535124536022401</v>
-      </c>
-      <c r="E19" s="9">
-        <f>SUM(Table13[[#This Row],[red leaves, temple and shrines]:[leisure activities]])</f>
-        <v>1.1788558731890761</v>
-      </c>
-    </row>
-    <row r="20" spans="1:5">
-      <c r="A20" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="B20" s="2">
-        <v>0.59753013079116402</v>
-      </c>
-      <c r="C20">
-        <v>0.33326031055897498</v>
-      </c>
-      <c r="D20" s="3">
-        <v>0.22469830162035301</v>
-      </c>
-      <c r="E20" s="9">
-        <f>SUM(Table13[[#This Row],[red leaves, temple and shrines]:[leisure activities]])</f>
-        <v>1.1554887429704921</v>
-      </c>
-    </row>
-    <row r="21" spans="1:5">
-      <c r="A21" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="B21" s="2">
-        <v>0.51750653091780496</v>
-      </c>
-      <c r="C21">
-        <v>0.36413314134936797</v>
-      </c>
-      <c r="D21" s="3">
-        <v>0.26376738507287201</v>
-      </c>
-      <c r="E21" s="9">
-        <f>SUM(Table13[[#This Row],[red leaves, temple and shrines]:[leisure activities]])</f>
-        <v>1.1454070573400448</v>
-      </c>
-    </row>
-    <row r="22" spans="1:5">
-      <c r="A22" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="B22" s="2">
-        <v>0.45841234955560201</v>
-      </c>
-      <c r="C22">
-        <v>0.42294676124438702</v>
-      </c>
-      <c r="D22" s="3">
-        <v>0.256194021047779</v>
-      </c>
-      <c r="E22" s="9">
-        <f>SUM(Table13[[#This Row],[red leaves, temple and shrines]:[leisure activities]])</f>
-        <v>1.1375531318477679</v>
-      </c>
-    </row>
-    <row r="23" spans="1:5">
-      <c r="A23" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="B23" s="2">
-        <v>0.531498341761096</v>
-      </c>
-      <c r="C23">
-        <v>0.287155135257879</v>
-      </c>
-      <c r="D23" s="3">
-        <v>0.30131542130644201</v>
-      </c>
-      <c r="E23" s="9">
-        <f>SUM(Table13[[#This Row],[red leaves, temple and shrines]:[leisure activities]])</f>
-        <v>1.119968898325417</v>
-      </c>
-    </row>
-    <row r="24" spans="1:5">
-      <c r="A24" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="B24" s="2">
-        <v>0.45001851657071301</v>
-      </c>
-      <c r="C24">
-        <v>0.32299738184833798</v>
-      </c>
-      <c r="D24" s="3">
-        <v>0.27088983565410402</v>
-      </c>
-      <c r="E24" s="9">
-        <f>SUM(Table13[[#This Row],[red leaves, temple and shrines]:[leisure activities]])</f>
-        <v>1.043905734073155</v>
-      </c>
-    </row>
-    <row r="25" spans="1:5" ht="30">
-      <c r="A25" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="B25" s="2">
-        <v>0.45363652525970799</v>
-      </c>
-      <c r="C25">
-        <v>0.33632613060500299</v>
-      </c>
-      <c r="D25" s="3">
-        <v>0.24358957396591799</v>
-      </c>
-      <c r="E25" s="9">
-        <f>SUM(Table13[[#This Row],[red leaves, temple and shrines]:[leisure activities]])</f>
-        <v>1.033552229830629</v>
-      </c>
-    </row>
-    <row r="26" spans="1:5">
-      <c r="A26" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="B26" s="2">
-        <v>0.37021656663841301</v>
-      </c>
-      <c r="C26">
-        <v>0.37660286969005002</v>
-      </c>
-      <c r="D26" s="3">
-        <v>0.27088983565410402</v>
-      </c>
-      <c r="E26" s="9">
-        <f>SUM(Table13[[#This Row],[red leaves, temple and shrines]:[leisure activities]])</f>
-        <v>1.0177092719825671</v>
-      </c>
-    </row>
-    <row r="27" spans="1:5">
-      <c r="A27" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="B27" s="2">
-        <v>0.54885801506965604</v>
-      </c>
-      <c r="C27">
-        <v>0.17606836507155399</v>
-      </c>
-      <c r="D27" s="3">
-        <v>0.280253857175909</v>
-      </c>
-      <c r="E27" s="9">
-        <f>SUM(Table13[[#This Row],[red leaves, temple and shrines]:[leisure activities]])</f>
-        <v>1.005180237317119</v>
-      </c>
-    </row>
-    <row r="28" spans="1:5" ht="30">
-      <c r="A28" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="B28" s="2">
-        <v>0.37002545176833201</v>
-      </c>
-      <c r="C28">
-        <v>0.30259155065307602</v>
-      </c>
-      <c r="D28" s="3">
-        <v>0.33085725393520099</v>
-      </c>
-      <c r="E28" s="9">
-        <f>SUM(Table13[[#This Row],[red leaves, temple and shrines]:[leisure activities]])</f>
-        <v>1.003474256356609</v>
-      </c>
-    </row>
-    <row r="29" spans="1:5">
-      <c r="A29" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="B29" s="2">
-        <v>0.54901529759286505</v>
-      </c>
-      <c r="C29">
-        <v>0.287155135257879</v>
-      </c>
-      <c r="D29" s="3">
-        <v>0.12535601227357501</v>
-      </c>
-      <c r="E29" s="9">
-        <f>SUM(Table13[[#This Row],[red leaves, temple and shrines]:[leisure activities]])</f>
-        <v>0.96152644512431906</v>
-      </c>
-    </row>
-    <row r="30" spans="1:5" ht="30">
-      <c r="A30" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="B30" s="2">
-        <v>0.74786406251777704</v>
-      </c>
-      <c r="C30">
-        <v>2.4466139546941199E-2</v>
-      </c>
-      <c r="D30" s="3">
-        <v>0.12535601227357501</v>
-      </c>
-      <c r="E30" s="9">
-        <f>SUM(Table13[[#This Row],[red leaves, temple and shrines]:[leisure activities]])</f>
-        <v>0.89768621433829332</v>
-      </c>
-    </row>
-    <row r="31" spans="1:5">
-      <c r="A31" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="B31" s="2">
-        <v>9.7541613744420802E-2</v>
-      </c>
-      <c r="C31">
-        <v>0.35772645010591703</v>
-      </c>
-      <c r="D31" s="3">
-        <v>0.28749173891801499</v>
-      </c>
-      <c r="E31" s="9">
-        <f>SUM(Table13[[#This Row],[red leaves, temple and shrines]:[leisure activities]])</f>
-        <v>0.74275980276835285</v>
-      </c>
-    </row>
-    <row r="32" spans="1:5">
-      <c r="A32" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="B32" s="2">
-        <v>0.37988430104084903</v>
-      </c>
-      <c r="C32">
-        <v>0.164487993682887</v>
-      </c>
-      <c r="D32" s="3">
-        <v>0.162020295483566</v>
-      </c>
-      <c r="E32" s="9">
-        <f>SUM(Table13[[#This Row],[red leaves, temple and shrines]:[leisure activities]])</f>
-        <v>0.70639259020730205</v>
-      </c>
-    </row>
-    <row r="33" spans="1:5">
-      <c r="A33" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="B33" s="2">
-        <v>0.44714418753246998</v>
-      </c>
-      <c r="C33">
-        <v>0.12652318558152101</v>
-      </c>
-      <c r="D33" s="3">
-        <v>9.93422893467788E-2</v>
-      </c>
-      <c r="E33" s="9">
-        <f>SUM(Table13[[#This Row],[red leaves, temple and shrines]:[leisure activities]])</f>
-        <v>0.67300966246076976</v>
-      </c>
-    </row>
-    <row r="34" spans="1:5">
-      <c r="A34" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="B34" s="2">
-        <v>0.29561788291983199</v>
-      </c>
-      <c r="C34">
-        <v>0.19150478046675101</v>
-      </c>
-      <c r="D34" s="3">
-        <v>0.18091156782913001</v>
-      </c>
-      <c r="E34" s="9">
-        <f>SUM(Table13[[#This Row],[red leaves, temple and shrines]:[leisure activities]])</f>
-        <v>0.66803423121571304</v>
-      </c>
-    </row>
-    <row r="35" spans="1:5">
-      <c r="A35" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="B35" s="2">
-        <v>0.39346805907529397</v>
-      </c>
-      <c r="C35">
-        <v>0.111086770186325</v>
-      </c>
-      <c r="D35" s="3">
-        <v>0.12535601227357501</v>
-      </c>
-      <c r="E35" s="9">
-        <f>SUM(Table13[[#This Row],[red leaves, temple and shrines]:[leisure activities]])</f>
-        <v>0.62991084153519394</v>
-      </c>
-    </row>
-    <row r="36" spans="1:5">
-      <c r="A36" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="B36" s="2">
-        <v>0.45060522810819598</v>
-      </c>
-      <c r="C36">
-        <v>1.54364153951964E-2</v>
-      </c>
-      <c r="D36" s="3">
-        <v>0.145533823380529</v>
-      </c>
-      <c r="E36" s="9">
-        <f>SUM(Table13[[#This Row],[red leaves, temple and shrines]:[leisure activities]])</f>
-        <v>0.61157546688392139</v>
-      </c>
-    </row>
-    <row r="37" spans="1:5">
-      <c r="A37" s="1" t="s">
+    <row r="38" spans="1:6">
+      <c r="A38">
         <v>37</v>
       </c>
-      <c r="B37" s="2">
+      <c r="B38" t="s">
+        <v>37</v>
+      </c>
+      <c r="C38">
         <v>0.30166363081053499</v>
       </c>
-      <c r="C37">
+      <c r="D38">
         <v>0</v>
       </c>
-      <c r="D37" s="3">
+      <c r="E38">
         <v>0</v>
       </c>
-      <c r="E37" s="9">
-        <f>SUM(Table13[[#This Row],[red leaves, temple and shrines]:[leisure activities]])</f>
+      <c r="F38">
         <v>0.30166363081053499</v>
       </c>
     </row>
-    <row r="38" spans="1:5">
-      <c r="A38" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="B38" s="2">
-        <v>0</v>
-      </c>
-      <c r="C38">
-        <v>0</v>
-      </c>
-      <c r="D38" s="3">
-        <v>6.2678006136787506E-2</v>
-      </c>
-      <c r="E38" s="9">
-        <f>SUM(Table13[[#This Row],[red leaves, temple and shrines]:[leisure activities]])</f>
-        <v>6.2678006136787506E-2</v>
-      </c>
-    </row>
   </sheetData>
-  <conditionalFormatting sqref="B2:D38">
+  <conditionalFormatting sqref="C2:E38">
+    <cfRule type="colorScale" priority="3">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FF63BE7B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FFF8696B"/>
+      </colorScale>
+    </cfRule>
     <cfRule type="colorScale" priority="2">
       <colorScale>
         <cfvo type="min"/>
@@ -5071,7 +5991,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E2:E38">
+  <conditionalFormatting sqref="F2:F38">
     <cfRule type="colorScale" priority="1">
       <colorScale>
         <cfvo type="min"/>

</xml_diff>